<commit_message>
Se modificaron la estrategia de seguimiento a las no confirmidades
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/1. Aseguramiento de la calidad/IWM_PlanAseguramientoCalidad.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/1. Aseguramiento de la calidad/IWM_PlanAseguramientoCalidad.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>Auditoria</t>
   </si>
@@ -25,15 +25,9 @@
     <t>Al finalizar la estimación y planeación</t>
   </si>
   <si>
-    <t>Ejecución</t>
-  </si>
-  <si>
     <t>Al finalizar la ejecución</t>
   </si>
   <si>
-    <t>Anualmente</t>
-  </si>
-  <si>
     <t>Auditor externo</t>
   </si>
   <si>
@@ -52,9 +46,6 @@
     <t>Plan de proyecto</t>
   </si>
   <si>
-    <t>Lista de no conformidades</t>
-  </si>
-  <si>
     <t>Responsable de ejecución</t>
   </si>
   <si>
@@ -70,18 +61,12 @@
     <t>Líder de proyecto</t>
   </si>
   <si>
-    <t>Auditorias a planes</t>
-  </si>
-  <si>
     <t>5 días</t>
   </si>
   <si>
     <t>Dirección</t>
   </si>
   <si>
-    <t>Auditorias anuales</t>
-  </si>
-  <si>
     <t>Al finalizar estimación y planeación</t>
   </si>
   <si>
@@ -106,18 +91,12 @@
     <t>Medición</t>
   </si>
   <si>
-    <t>Seguimiento del proyecto</t>
-  </si>
-  <si>
     <t>Mensual</t>
   </si>
   <si>
     <t>Líder de procesos</t>
   </si>
   <si>
-    <t>Responsable de Aseguramiento de la calidad</t>
-  </si>
-  <si>
     <t>Ariana Sosa</t>
   </si>
   <si>
@@ -148,18 +127,6 @@
     <t>Plan de Mejora</t>
   </si>
   <si>
-    <t>Responsable de Entrenamiento</t>
-  </si>
-  <si>
-    <t>Estimación y Planeación</t>
-  </si>
-  <si>
-    <t>Entrega con el Cliente</t>
-  </si>
-  <si>
-    <t>Toma de Decisión</t>
-  </si>
-  <si>
     <t>Cuando se ejecute el proceso</t>
   </si>
   <si>
@@ -172,16 +139,55 @@
     <t>Aseguramiento de la Calidad</t>
   </si>
   <si>
-    <t>Físicas</t>
-  </si>
-  <si>
-    <t>Funcionales</t>
-  </si>
-  <si>
     <t>Cambios</t>
   </si>
   <si>
     <t>Cuando ocurra</t>
+  </si>
+  <si>
+    <t>Requerimientos, Fisica y Funcional</t>
+  </si>
+  <si>
+    <t>Estimación y Planeación, Fisica y Funcional</t>
+  </si>
+  <si>
+    <t>Ejecución, Fisica y Funcional</t>
+  </si>
+  <si>
+    <t>Entrega con el Cliente, Fisica y Funcional</t>
+  </si>
+  <si>
+    <t>Seguimiento del proyecto, Fisica y Funcional</t>
+  </si>
+  <si>
+    <t>Toma de Decisión, Fisica y Funcional</t>
+  </si>
+  <si>
+    <t>Semestral</t>
+  </si>
+  <si>
+    <t>Momento de Ejecución</t>
+  </si>
+  <si>
+    <t>Procesos</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Fisicas y Funcionales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Líder de mejora </t>
+  </si>
+  <si>
+    <t>Líder de Procesos, Líder de Proyectos</t>
+  </si>
+  <si>
+    <t>Encargado de RH</t>
+  </si>
+  <si>
+    <t>Líder de Procesos, Líder de Proyectos, Aseguramiento de la Calidad, Encargado de RH</t>
   </si>
 </sst>
 </file>
@@ -306,7 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -320,8 +326,8 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -331,9 +337,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -680,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:D42"/>
+  <dimension ref="A5:D40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D22"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,7 +719,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -730,431 +733,409 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="C20" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>23</v>
+      <c r="C26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="C32" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="2" t="s">
+      <c r="A37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="2" t="s">
+    </row>
+    <row r="38" spans="1:4" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A5:D6"/>
     <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se actualizo la parte de productos
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/1. Aseguramiento de la calidad/IWM_PlanAseguramientoCalidad.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/1. Aseguramiento de la calidad/IWM_PlanAseguramientoCalidad.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
   <si>
     <t>Auditoria</t>
   </si>
@@ -188,6 +188,15 @@
   </si>
   <si>
     <t>Líder de Procesos, Líder de Proyectos, Aseguramiento de la Calidad, Encargado de RH</t>
+  </si>
+  <si>
+    <t>Analisis y Diseño</t>
+  </si>
+  <si>
+    <t>Casos de Pruebas</t>
+  </si>
+  <si>
+    <t>Entrega Proyecto</t>
   </si>
 </sst>
 </file>
@@ -683,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:D40"/>
+  <dimension ref="A5:D43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,7 +759,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
@@ -778,7 +787,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
@@ -932,7 +941,7 @@
         <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -979,91 +988,91 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>49</v>
@@ -1072,62 +1081,104 @@
         <v>27</v>
       </c>
       <c r="D35" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+    <row r="41" spans="1:4" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+    <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>